<commit_message>
Casi terminado para ver empate
</commit_message>
<xml_diff>
--- a/Codigo de colores.xlsx
+++ b/Codigo de colores.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\UVG\Semestre 3\Org. Computadoras y Assembler\Proyecto 2\Circuitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose\Desktop\DISEÑO\TRABAJOS\UVG\3er Semestre\Assembler\Proyecto 2\Final\Proyecto-Assembler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14976" windowHeight="5748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14970" windowHeight="5745"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Color</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>Posiciones</t>
+  </si>
+  <si>
+    <t>Morado nena</t>
+  </si>
+  <si>
+    <t>Entrada de ors para ver si hay empate</t>
+  </si>
+  <si>
+    <t>Morado casi negro</t>
+  </si>
+  <si>
+    <t>Entradas or para ver si alguien gano</t>
   </si>
 </sst>
 </file>
@@ -188,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +273,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B144C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -566,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,34 +603,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -659,6 +662,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,6 +697,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3B144C"/>
       <color rgb="FF666633"/>
       <color rgb="FF777777"/>
       <color rgb="FF00FF00"/>
@@ -951,66 +982,66 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="10" t="s">
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="I1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="26" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="29">
         <v>3</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -1023,21 +1054,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="11">
         <v>4</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>5</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="30">
         <v>6</v>
       </c>
       <c r="I4" s="3">
@@ -1050,21 +1081,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="31">
         <v>7</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="32">
         <v>8</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>9</v>
       </c>
       <c r="I5" s="3">
@@ -1077,12 +1108,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="34" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="27" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="3">
@@ -1095,12 +1126,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="27" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="3">
@@ -1113,12 +1144,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="27" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="3">
@@ -1131,12 +1162,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="34" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="27" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="3">
@@ -1149,12 +1180,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="34" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="27" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="3">
@@ -1167,12 +1198,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="27" t="s">
         <v>44</v>
       </c>
       <c r="I11" s="3">
@@ -1185,12 +1216,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="35" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="28" t="s">
         <v>45</v>
       </c>
       <c r="I12" s="3">
@@ -1203,11 +1234,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L18" s="4"/>
     </row>
   </sheetData>

</xml_diff>